<commit_message>
Update with Correct Forecast output
</commit_message>
<xml_diff>
--- a/4_week_report.xlsx
+++ b/4_week_report.xlsx
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>784.5</v>
+        <v>784</v>
       </c>
       <c r="D3" t="n">
         <v>1055</v>
@@ -644,7 +644,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>597.5999999999999</v>
+        <v>597.0999999999999</v>
       </c>
       <c r="D8" t="n">
         <v>571</v>
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>411.3</v>
+        <v>408.8</v>
       </c>
       <c r="D12" t="n">
         <v>541</v>
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2641.1</v>
+        <v>2631.6</v>
       </c>
       <c r="D14" t="n">
         <v>2460</v>
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>191.7</v>
+        <v>198.6</v>
       </c>
       <c r="D15" t="n">
         <v>160</v>
@@ -914,7 +914,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>30.1</v>
+        <v>29.85</v>
       </c>
       <c r="D18" t="n">
         <v>25</v>
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>656.8</v>
+        <v>652.3</v>
       </c>
       <c r="D20" t="n">
         <v>648</v>
@@ -1076,7 +1076,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>828.9</v>
+        <v>829.9</v>
       </c>
       <c r="D24" t="n">
         <v>1208</v>
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>160.9</v>
+        <v>160.4</v>
       </c>
       <c r="D27" t="n">
         <v>95</v>
@@ -1211,7 +1211,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>11</v>
+        <v>9.600000000000001</v>
       </c>
       <c r="D29" t="n">
         <v>16</v>
@@ -1238,7 +1238,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>518.5</v>
+        <v>517.5</v>
       </c>
       <c r="D30" t="n">
         <v>644</v>
@@ -1265,7 +1265,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>741.1</v>
+        <v>743.1</v>
       </c>
       <c r="D31" t="n">
         <v>754</v>
@@ -1427,7 +1427,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2612.3</v>
+        <v>2631.3</v>
       </c>
       <c r="D37" t="n">
         <v>2695</v>
@@ -1454,7 +1454,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="D38" t="n">
         <v>8</v>
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>99.84999999999999</v>
+        <v>99.34999999999999</v>
       </c>
       <c r="D41" t="n">
         <v>73</v>
@@ -1643,7 +1643,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>9.999999999999998</v>
+        <v>9.499999999999998</v>
       </c>
       <c r="D45" t="n">
         <v>8</v>
@@ -1724,7 +1724,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>673.4999999999999</v>
+        <v>675.4999999999999</v>
       </c>
       <c r="D48" t="n">
         <v>673</v>
@@ -1805,7 +1805,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>268.5</v>
+        <v>261</v>
       </c>
       <c r="D51" t="n">
         <v>265</v>
@@ -2021,7 +2021,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>180.8</v>
+        <v>181.3</v>
       </c>
       <c r="D59" t="n">
         <v>184</v>
@@ -2048,7 +2048,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>280.9</v>
+        <v>276.9</v>
       </c>
       <c r="D60" t="n">
         <v>276</v>
@@ -2129,7 +2129,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>116.75</v>
+        <v>117.25</v>
       </c>
       <c r="D63" t="n">
         <v>48</v>
@@ -2237,7 +2237,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>328.8</v>
+        <v>325.8</v>
       </c>
       <c r="D67" t="n">
         <v>281</v>
@@ -2264,7 +2264,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>162.8</v>
+        <v>161.8</v>
       </c>
       <c r="D68" t="n">
         <v>139</v>
@@ -2345,7 +2345,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>302.5</v>
+        <v>297.5</v>
       </c>
       <c r="D71" t="n">
         <v>242</v>
@@ -2399,7 +2399,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>169.8</v>
+        <v>168.8</v>
       </c>
       <c r="D73" t="n">
         <v>177</v>
@@ -2561,7 +2561,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>73.2</v>
+        <v>72.2</v>
       </c>
       <c r="D79" t="n">
         <v>70</v>
@@ -2588,7 +2588,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>89.10000000000001</v>
+        <v>88.10000000000001</v>
       </c>
       <c r="D80" t="n">
         <v>81</v>
@@ -2615,7 +2615,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>221</v>
+        <v>217.5</v>
       </c>
       <c r="D81" t="n">
         <v>257</v>
@@ -2642,7 +2642,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>2735.400000000001</v>
+        <v>2735.900000000001</v>
       </c>
       <c r="D82" t="n">
         <v>3404</v>
@@ -2669,7 +2669,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>101.3</v>
+        <v>98.29999999999998</v>
       </c>
       <c r="D83" t="n">
         <v>87</v>
@@ -2750,7 +2750,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>183.7</v>
+        <v>183.2</v>
       </c>
       <c r="D86" t="n">
         <v>163</v>
@@ -2858,7 +2858,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>427.9999999999999</v>
+        <v>427.4999999999999</v>
       </c>
       <c r="D90" t="n">
         <v>564</v>
@@ -3263,7 +3263,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>139.1</v>
+        <v>138.6</v>
       </c>
       <c r="D105" t="n">
         <v>157</v>

</xml_diff>

<commit_message>
Update (Analyze PO & Forecast)
</commit_message>
<xml_diff>
--- a/4_week_report.xlsx
+++ b/4_week_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G141"/>
+  <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4.56</v>
+        <v>4.460000000000001</v>
       </c>
       <c r="D2" t="n">
         <v>16</v>
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>718.5</v>
+        <v>711.5</v>
       </c>
       <c r="D3" t="n">
         <v>575</v>
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.8</v>
+        <v>3.73</v>
       </c>
       <c r="D4" t="n">
         <v>4</v>
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.22</v>
+        <v>1.46</v>
       </c>
       <c r="D6" t="n">
         <v>7</v>
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>486.2</v>
+        <v>449</v>
       </c>
       <c r="D9" t="n">
         <v>374</v>
@@ -716,694 +716,700 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>B08KWMXGQW</t>
+          <t>B08LGKGBKT</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>B450M DS3H V2</t>
+          <t>B550 GAMING X V2</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>771.8000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>651</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>785</v>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>935</v>
       </c>
       <c r="G11" t="n">
-        <v>4</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>B08LGKGBKT</t>
+          <t>B089FY7QT1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>B550 GAMING X V2</t>
+          <t>B550M DS3H</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>770.8000000000001</v>
+        <v>4.32</v>
       </c>
       <c r="D12" t="n">
-        <v>651</v>
+        <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>785</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
-        <v>935</v>
+        <v>18</v>
       </c>
       <c r="G12" t="n">
-        <v>1171</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>B089FY7QT1</t>
+          <t>B07GBM3M88</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>B550M DS3H</t>
+          <t>GC-WB1733D-I</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4.32</v>
+        <v>9.920000000000002</v>
       </c>
       <c r="D13" t="n">
         <v>12</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
         <v>18</v>
       </c>
       <c r="G13" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>B07GBM3M88</t>
+          <t>B091HTG6DQ</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GC-WB1733D-I</t>
+          <t>GC-WBAX210</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9.920000000000002</v>
+        <v>2423</v>
       </c>
       <c r="D14" t="n">
-        <v>12</v>
+        <v>2394</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>2609</v>
       </c>
       <c r="F14" t="n">
-        <v>18</v>
+        <v>2763</v>
       </c>
       <c r="G14" t="n">
-        <v>24</v>
+        <v>2987</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>B091HTG6DQ</t>
+          <t>B07VNBC5PS</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>GC-WBAX210</t>
+          <t>GC-WBAX200</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2395</v>
+        <v>159</v>
       </c>
       <c r="D15" t="n">
-        <v>2394</v>
+        <v>143</v>
       </c>
       <c r="E15" t="n">
-        <v>2609</v>
+        <v>174</v>
       </c>
       <c r="F15" t="n">
-        <v>2763</v>
+        <v>201</v>
       </c>
       <c r="G15" t="n">
-        <v>2987</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>B07VNBC5PS</t>
+          <t>B0BF73P6HY</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>GC-WBAX200</t>
+          <t>X670E AORUS XTREME</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>111</v>
+        <v>4.42</v>
       </c>
       <c r="D16" t="n">
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="E16" t="n">
-        <v>174</v>
+        <v>22</v>
       </c>
       <c r="F16" t="n">
-        <v>201</v>
+        <v>31</v>
       </c>
       <c r="G16" t="n">
-        <v>246</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>B0BF73P6HY</t>
+          <t>B083NN4MLZ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>X670E AORUS XTREME</t>
+          <t>Z690 AERO G</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3.82</v>
+        <v>0.5599999999999999</v>
       </c>
       <c r="D17" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E17" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="G17" t="n">
-        <v>45</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>B083NN4MLZ</t>
+          <t>B0BH9BBLHB</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Z690 AERO G</t>
+          <t>Z790 AERO G</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.5599999999999999</v>
+        <v>17.74</v>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F18" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G18" t="n">
-        <v>8</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>B0BH9BBLHB</t>
+          <t>B0BHTMXMRQ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Z790 AERO G</t>
+          <t>Z790 UD AC</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>17.74</v>
+        <v>176</v>
       </c>
       <c r="D19" t="n">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="E19" t="n">
-        <v>24</v>
+        <v>229</v>
       </c>
       <c r="F19" t="n">
-        <v>30</v>
+        <v>265</v>
       </c>
       <c r="G19" t="n">
-        <v>41</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>B0BHTMXMRQ</t>
+          <t>B07FWVJSHC</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Z790 UD AC</t>
+          <t>B450M DS3H</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>227</v>
+        <v>2.32</v>
       </c>
       <c r="D20" t="n">
-        <v>191</v>
+        <v>8</v>
       </c>
       <c r="E20" t="n">
-        <v>229</v>
+        <v>8</v>
       </c>
       <c r="F20" t="n">
-        <v>265</v>
+        <v>12</v>
       </c>
       <c r="G20" t="n">
-        <v>324</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>B07FWVJSHC</t>
+          <t>B08F7BHDLY</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>B450M DS3H</t>
+          <t>A520I AC</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2.32</v>
+        <v>464</v>
       </c>
       <c r="D21" t="n">
-        <v>8</v>
+        <v>407</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>470</v>
       </c>
       <c r="F21" t="n">
-        <v>12</v>
+        <v>524</v>
       </c>
       <c r="G21" t="n">
-        <v>24</v>
+        <v>606</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>B08F7BHDLY</t>
+          <t>B07FW85VFT</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>A520I AC</t>
+          <t>B450 AORUS PRO WIFI</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>468</v>
+        <v>6.800000000000001</v>
       </c>
       <c r="D22" t="n">
-        <v>407</v>
+        <v>28</v>
       </c>
       <c r="E22" t="n">
-        <v>470</v>
+        <v>31</v>
       </c>
       <c r="F22" t="n">
-        <v>524</v>
+        <v>47</v>
       </c>
       <c r="G22" t="n">
-        <v>606</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>B07FW85VFT</t>
+          <t>B08B7ZX8Q2</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>B450 AORUS PRO WIFI</t>
+          <t>B450M DS3H WIFI</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.800000000000001</v>
+        <v>441.6000000000001</v>
       </c>
       <c r="D23" t="n">
-        <v>28</v>
+        <v>626</v>
       </c>
       <c r="E23" t="n">
-        <v>31</v>
+        <v>756</v>
       </c>
       <c r="F23" t="n">
-        <v>47</v>
+        <v>901</v>
       </c>
       <c r="G23" t="n">
-        <v>79</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>B08B7ZX8Q2</t>
+          <t>B08WPV5HS7</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>B450M DS3H WIFI</t>
+          <t>Z590 AORUS ELITE</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>441.6000000000001</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>626</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>756</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>901</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>1128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>B08WPV5HS7</t>
+          <t>B09J5TC4F8</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Z590 AORUS ELITE</t>
+          <t>Z690 GAMING X DDR4</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>0.5599999999999999</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="E25" t="n">
+        <v>4</v>
+      </c>
+      <c r="F25" t="n">
+        <v>8</v>
+      </c>
+      <c r="G25" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>B09J5TC4F8</t>
+          <t>B0BH9DXY38</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Z690 GAMING X DDR4</t>
+          <t>Z790 AORUS ELITE AX</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.5599999999999999</v>
+        <v>1073.9</v>
       </c>
       <c r="D26" t="n">
-        <v>4</v>
+        <v>934</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>1094</v>
       </c>
       <c r="F26" t="n">
-        <v>8</v>
+        <v>1241</v>
       </c>
       <c r="G26" t="n">
-        <v>17</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>B0BH9DXY38</t>
+          <t>B079NYQQJJ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Z790 AORUS ELITE AX</t>
+          <t>GA-A320M-S2H</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1214.2</v>
+        <v>1.12</v>
       </c>
       <c r="D27" t="n">
-        <v>934</v>
+        <v>8</v>
       </c>
       <c r="E27" t="n">
-        <v>1094</v>
+        <v>8</v>
       </c>
       <c r="F27" t="n">
-        <v>1241</v>
+        <v>12</v>
       </c>
       <c r="G27" t="n">
-        <v>1466</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>B079NYQQJJ</t>
+          <t>B08F7HPJ4F</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>GA-A320M-S2H</t>
+          <t>A520M S2H</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1.12</v>
+        <v>677.3000000000001</v>
       </c>
       <c r="D28" t="n">
-        <v>8</v>
+        <v>521</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>629</v>
       </c>
       <c r="F28" t="n">
-        <v>12</v>
+        <v>742</v>
       </c>
       <c r="G28" t="n">
-        <v>24</v>
+        <v>919</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>B08F7HPJ4F</t>
+          <t>B089FWWN62</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>A520M S2H</t>
+          <t>B550I AORUS PRO AX</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>677.3000000000001</v>
+        <v>52.66</v>
       </c>
       <c r="D29" t="n">
-        <v>521</v>
+        <v>163</v>
       </c>
       <c r="E29" t="n">
-        <v>629</v>
+        <v>197</v>
       </c>
       <c r="F29" t="n">
-        <v>742</v>
+        <v>235</v>
       </c>
       <c r="G29" t="n">
-        <v>919</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>B089FWWN62</t>
+          <t>B0BH9F7DKS</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>B550I AORUS PRO AX</t>
+          <t>Z790 AORUS MASTER</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>52.26000000000001</v>
+        <v>91.00000000000001</v>
       </c>
       <c r="D30" t="n">
-        <v>163</v>
+        <v>70</v>
       </c>
       <c r="E30" t="n">
-        <v>197</v>
+        <v>86</v>
       </c>
       <c r="F30" t="n">
-        <v>235</v>
+        <v>112</v>
       </c>
       <c r="G30" t="n">
-        <v>295</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>B0BH9F7DKS</t>
+          <t>B07WL5MFXL</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Z790 AORUS MASTER</t>
+          <t>X570 AORUS ELITE WIFI</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>91.00000000000001</v>
+        <v>4.4</v>
       </c>
       <c r="D31" t="n">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="E31" t="n">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="F31" t="n">
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="G31" t="n">
-        <v>153</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>B07WL5MFXL</t>
+          <t>B0BSB6MB15</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>X570 AORUS ELITE WIFI</t>
+          <t>B760M DS3H DDR4</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>4.4</v>
+        <v>755.3</v>
       </c>
       <c r="D32" t="n">
-        <v>8</v>
+        <v>581</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>678</v>
       </c>
       <c r="F32" t="n">
-        <v>16</v>
+        <v>766</v>
       </c>
       <c r="G32" t="n">
-        <v>28</v>
+        <v>899</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>B0BSB6MB15</t>
+          <t>B0BF7FT26Z</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>B760M DS3H DDR4</t>
+          <t>X670 AORUS ELITE AX</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>755.3</v>
+        <v>616.2</v>
       </c>
       <c r="D33" t="n">
-        <v>581</v>
+        <v>474</v>
       </c>
       <c r="E33" t="n">
-        <v>678</v>
+        <v>559</v>
       </c>
       <c r="F33" t="n">
-        <v>766</v>
+        <v>639</v>
       </c>
       <c r="G33" t="n">
-        <v>899</v>
+        <v>761</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>B0BF7FT26Z</t>
+          <t>B0BF7CL99N</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>X670 AORUS ELITE AX</t>
+          <t>X670E AORUS MASTER</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>616.2</v>
+        <v>12.88</v>
       </c>
       <c r="D34" t="n">
-        <v>474</v>
+        <v>48</v>
       </c>
       <c r="E34" t="n">
-        <v>559</v>
+        <v>60</v>
       </c>
       <c r="F34" t="n">
-        <v>639</v>
+        <v>79</v>
       </c>
       <c r="G34" t="n">
-        <v>761</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>B0BF7CL99N</t>
+          <t>B07HS59X7P</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>X670E AORUS MASTER</t>
+          <t>Z390 UD</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>12.88</v>
+        <v>0.14</v>
       </c>
       <c r="D35" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>79</v>
+        <v>2</v>
       </c>
       <c r="G35" t="n">
-        <v>109</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>B07HS59X7P</t>
+          <t>B083GT6ZBX</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Z390 UD</t>
+          <t>Z590 AORUS TACHYON</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.14</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G36" t="n">
         <v>4</v>
@@ -1412,313 +1418,313 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>B083GT6ZBX</t>
+          <t>B08BR1XDX5</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Z590 AORUS TACHYON</t>
+          <t>B550M AORUS ELITE</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F37" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="G37" t="n">
-        <v>4</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>B08BR1XDX5</t>
+          <t>B0BH79FMW3</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>B550M AORUS ELITE</t>
+          <t>B650 AERO G</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2.8</v>
+        <v>49.2</v>
       </c>
       <c r="D38" t="n">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="E38" t="n">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="F38" t="n">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="G38" t="n">
-        <v>51</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>B0BH79FMW3</t>
+          <t>B0BH7GTY9C</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>B650 AERO G</t>
+          <t>B650 AORUS ELITE AX</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>48.2</v>
+        <v>2554.5</v>
       </c>
       <c r="D39" t="n">
-        <v>54</v>
+        <v>1965</v>
       </c>
       <c r="E39" t="n">
-        <v>66</v>
+        <v>2293</v>
       </c>
       <c r="F39" t="n">
-        <v>79</v>
+        <v>2587</v>
       </c>
       <c r="G39" t="n">
-        <v>99</v>
+        <v>3031</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>B0BH7GTY9C</t>
+          <t>B0BJ5SDGXK</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>B650 AORUS ELITE AX</t>
+          <t>B660M A ELITE AX DDR4</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2554.5</v>
+        <v>0.5599999999999999</v>
       </c>
       <c r="D40" t="n">
-        <v>1965</v>
+        <v>4</v>
       </c>
       <c r="E40" t="n">
-        <v>2293</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
-        <v>2587</v>
+        <v>8</v>
       </c>
       <c r="G40" t="n">
-        <v>3031</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>B0BJ5SDGXK</t>
+          <t>B0BSB4TYHV</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>B660M A ELITE AX DDR4</t>
+          <t>B760M AORUS ELITE AX</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.5599999999999999</v>
+        <v>3.34</v>
       </c>
       <c r="D41" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F41" t="n">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="G41" t="n">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>B0BSB4TYHV</t>
+          <t>B087GH5SK2</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>B760M AORUS ELITE AX</t>
+          <t>Z490 AORUS MASTER</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>3.34</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="G42" t="n">
-        <v>62</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>B087GH5SK2</t>
+          <t>B0BSVYXM5C</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Z490 AORUS MASTER</t>
+          <t>Z790 GAMING X AX</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>41.3</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="F43" t="n">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="G43" t="n">
-        <v>2</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>B0BSVYXM5C</t>
+          <t>B0BSNYN4XQ</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Z790 GAMING X AX</t>
+          <t>B760 DS3H AC DDR4</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>41.3</v>
+        <v>66.3</v>
       </c>
       <c r="D44" t="n">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E44" t="n">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="F44" t="n">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="G44" t="n">
-        <v>124</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>B0BSNYN4XQ</t>
+          <t>B0BVWQ3BMJ</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>B760 DS3H AC DDR4</t>
+          <t>B760I AORUS PRO DDR4</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>66.3</v>
+        <v>12.72</v>
       </c>
       <c r="D45" t="n">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="E45" t="n">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="F45" t="n">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="G45" t="n">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>B0BVWQ3BMJ</t>
+          <t>B0BSP61QZC</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>B760I AORUS PRO DDR4</t>
+          <t>B760M DS3H AX</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>12.72</v>
+        <v>443.3</v>
       </c>
       <c r="D46" t="n">
-        <v>32</v>
+        <v>341</v>
       </c>
       <c r="E46" t="n">
-        <v>37</v>
+        <v>398</v>
       </c>
       <c r="F46" t="n">
-        <v>56</v>
+        <v>449</v>
       </c>
       <c r="G46" t="n">
-        <v>89</v>
+        <v>526</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>B0BSP61QZC</t>
+          <t>B083R7SWF5</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>B760M DS3H AX</t>
+          <t>B760M DS3H AX DDR4</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>443.3</v>
+        <v>1.48</v>
       </c>
       <c r="D47" t="n">
-        <v>341</v>
+        <v>8</v>
       </c>
       <c r="E47" t="n">
-        <v>398</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
-        <v>449</v>
+        <v>12</v>
       </c>
       <c r="G47" t="n">
-        <v>526</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>B083R7SWF5</t>
+          <t>B09J6BWK2Z</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>B760M DS3H AX DDR4</t>
+          <t>Z690 AORUS ELITE AX DDR4</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1.48</v>
+        <v>3.44</v>
       </c>
       <c r="D48" t="n">
         <v>8</v>
@@ -1727,2426 +1733,2468 @@
         <v>8</v>
       </c>
       <c r="F48" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G48" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>B09J6BWK2Z</t>
+          <t>B0BTQ3SVFR</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Z690 AORUS ELITE AX DDR4</t>
+          <t>B550 UD AC</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3.44</v>
+        <v>57.36</v>
       </c>
       <c r="D49" t="n">
-        <v>8</v>
+        <v>186</v>
       </c>
       <c r="E49" t="n">
-        <v>8</v>
+        <v>228</v>
       </c>
       <c r="F49" t="n">
-        <v>16</v>
+        <v>289</v>
       </c>
       <c r="G49" t="n">
-        <v>29</v>
+        <v>391</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>B0BTQ3SVFR</t>
+          <t>B0BTTZFQTP</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>B550 UD AC</t>
+          <t>B550M K</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>58.16000000000001</v>
+        <v>873.6</v>
       </c>
       <c r="D50" t="n">
-        <v>186</v>
+        <v>672</v>
       </c>
       <c r="E50" t="n">
-        <v>228</v>
+        <v>796</v>
       </c>
       <c r="F50" t="n">
-        <v>289</v>
+        <v>916</v>
       </c>
       <c r="G50" t="n">
-        <v>391</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>B0BTTZFQTP</t>
+          <t>B07STNZF9L</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>B550M K</t>
+          <t>X570 AORUS PRO WIFI</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>873.6</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>796</v>
+        <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>916</v>
+        <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>1103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>B07STNZF9L</t>
+          <t>B0BVBXT6P1</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>X570 AORUS PRO WIFI</t>
+          <t>H610M S2H V2 DDR4</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
+        <v>206</v>
+      </c>
+      <c r="E52" t="n">
+        <v>244</v>
+      </c>
+      <c r="F52" t="n">
+        <v>284</v>
+      </c>
+      <c r="G52" t="n">
+        <v>344</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>B0BVBXT6P1</t>
+          <t>B083R7PHMX</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>H610M S2H V2 DDR4</t>
+          <t>Z790 D DDR4</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>209</v>
+        <v>2.08</v>
       </c>
       <c r="D53" t="n">
-        <v>206</v>
+        <v>8</v>
       </c>
       <c r="E53" t="n">
-        <v>244</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
-        <v>284</v>
+        <v>12</v>
       </c>
       <c r="G53" t="n">
-        <v>344</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>B083R7PHMX</t>
+          <t>B083R826VW</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Z790 D DDR4</t>
+          <t>B650I AORUS ULTRA</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>2.08</v>
+        <v>196.6</v>
       </c>
       <c r="D54" t="n">
-        <v>8</v>
+        <v>189</v>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>225</v>
       </c>
       <c r="F54" t="n">
-        <v>12</v>
+        <v>261</v>
       </c>
       <c r="G54" t="n">
-        <v>21</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>B083R826VW</t>
+          <t>B0BSB6MZ2L</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>B650I AORUS ULTRA</t>
+          <t>B760 AORUS ELITE AX</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>179</v>
+        <v>136.5</v>
       </c>
       <c r="D55" t="n">
-        <v>189</v>
+        <v>105</v>
       </c>
       <c r="E55" t="n">
-        <v>225</v>
+        <v>128</v>
       </c>
       <c r="F55" t="n">
-        <v>261</v>
+        <v>154</v>
       </c>
       <c r="G55" t="n">
-        <v>317</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>B0BSB6MZ2L</t>
+          <t>B083R7T5P4</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>B760 AORUS ELITE AX</t>
+          <t>Z790 UD AX</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>136.5</v>
+        <v>1.64</v>
       </c>
       <c r="D56" t="n">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="E56" t="n">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="F56" t="n">
-        <v>154</v>
+        <v>12</v>
       </c>
       <c r="G56" t="n">
-        <v>197</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>B083R7T5P4</t>
+          <t>B0BZQ43XXL</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Z790 UD AX</t>
+          <t>Z790I AORUS ULTRA</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1.64</v>
+        <v>13.34</v>
       </c>
       <c r="D57" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F57" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G57" t="n">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>B0BZQ43XXL</t>
+          <t>B09J64TBJG</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Z790I AORUS ULTRA</t>
+          <t>Z690 AORUS MASTER</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>13.34</v>
+        <v>1.12</v>
       </c>
       <c r="D58" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E58" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="F58" t="n">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="G58" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>B09J64TBJG</t>
+          <t>B0BYBHW4SH</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Z690 AORUS MASTER</t>
+          <t>B650 GAMING X AX</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1.12</v>
+        <v>503.1</v>
       </c>
       <c r="D59" t="n">
-        <v>8</v>
+        <v>387</v>
       </c>
       <c r="E59" t="n">
-        <v>4</v>
+        <v>468</v>
       </c>
       <c r="F59" t="n">
-        <v>12</v>
+        <v>553</v>
       </c>
       <c r="G59" t="n">
-        <v>20</v>
+        <v>688</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>B0BYBHW4SH</t>
+          <t>B0BZ54DR5L</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>B650 GAMING X AX</t>
+          <t>B760 GAMING X AX</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>503.1</v>
+        <v>69.8</v>
       </c>
       <c r="D60" t="n">
-        <v>387</v>
+        <v>66</v>
       </c>
       <c r="E60" t="n">
-        <v>468</v>
+        <v>80</v>
       </c>
       <c r="F60" t="n">
-        <v>553</v>
+        <v>102</v>
       </c>
       <c r="G60" t="n">
-        <v>688</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>B0BZ54DR5L</t>
+          <t>B0C4CKCRYW</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>B760 GAMING X AX</t>
+          <t>B760I AORUS PRO</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>67.59999999999999</v>
+        <v>57.2</v>
       </c>
       <c r="D61" t="n">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="E61" t="n">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="F61" t="n">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="G61" t="n">
-        <v>132</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>B0C4CKCRYW</t>
+          <t>B0BZQ1PWGJ</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>B760I AORUS PRO</t>
+          <t>B760M C</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>57.2</v>
+        <v>189.8</v>
       </c>
       <c r="D62" t="n">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="E62" t="n">
-        <v>56</v>
+        <v>177</v>
       </c>
       <c r="F62" t="n">
-        <v>70</v>
+        <v>214</v>
       </c>
       <c r="G62" t="n">
-        <v>93</v>
+        <v>270</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>B0BZQ1PWGJ</t>
+          <t>B0BZQ1TNW8</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>B760M C</t>
+          <t>B550M AORUS ELITE AX</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>189.8</v>
+        <v>256.3</v>
       </c>
       <c r="D63" t="n">
-        <v>146</v>
+        <v>315</v>
       </c>
       <c r="E63" t="n">
-        <v>177</v>
+        <v>382</v>
       </c>
       <c r="F63" t="n">
-        <v>214</v>
+        <v>455</v>
       </c>
       <c r="G63" t="n">
-        <v>270</v>
+        <v>569</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>B0BZQ1TNW8</t>
+          <t>B0C1M2BDNR</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>B550M AORUS ELITE AX</t>
+          <t>Q670M D3H</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>256.3</v>
+        <v>4.800000000000001</v>
       </c>
       <c r="D64" t="n">
-        <v>315</v>
+        <v>8</v>
       </c>
       <c r="E64" t="n">
-        <v>382</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
-        <v>455</v>
+        <v>12</v>
       </c>
       <c r="G64" t="n">
-        <v>569</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>B0C1M2BDNR</t>
+          <t>B0C4CKFV65</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Q670M D3H</t>
+          <t>A620M S2H</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>4.800000000000001</v>
+        <v>127.9</v>
       </c>
       <c r="D65" t="n">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>123</v>
       </c>
       <c r="F65" t="n">
-        <v>12</v>
+        <v>150</v>
       </c>
       <c r="G65" t="n">
-        <v>16</v>
+        <v>191</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>B0C4CKFV65</t>
+          <t>B0BZ17BQ4Z</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>A620M S2H</t>
+          <t>B650M K</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>127.9</v>
+        <v>15.04</v>
       </c>
       <c r="D66" t="n">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="E66" t="n">
-        <v>123</v>
+        <v>47</v>
       </c>
       <c r="F66" t="n">
-        <v>150</v>
+        <v>74</v>
       </c>
       <c r="G66" t="n">
-        <v>191</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>B0BZ17BQ4Z</t>
+          <t>B0C4CB8G8D</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>B650M K</t>
+          <t>H610I</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>15.04</v>
+        <v>148.2</v>
       </c>
       <c r="D67" t="n">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="E67" t="n">
-        <v>47</v>
+        <v>136</v>
       </c>
       <c r="F67" t="n">
-        <v>74</v>
+        <v>158</v>
       </c>
       <c r="G67" t="n">
-        <v>125</v>
+        <v>195</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>B0C4CB8G8D</t>
+          <t>B0BZQ416QM</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>H610I</t>
+          <t>H610M S2H</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>148.2</v>
+        <v>191.1</v>
       </c>
       <c r="D68" t="n">
-        <v>114</v>
+        <v>147</v>
       </c>
       <c r="E68" t="n">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="F68" t="n">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="G68" t="n">
-        <v>195</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>B0BZQ416QM</t>
+          <t>B0C1ZZ57ZW</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>H610M S2H</t>
+          <t>A620M GAMING X</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>166</v>
+        <v>4.42</v>
       </c>
       <c r="D69" t="n">
-        <v>147</v>
+        <v>17</v>
       </c>
       <c r="E69" t="n">
-        <v>172</v>
+        <v>12</v>
       </c>
       <c r="F69" t="n">
-        <v>197</v>
+        <v>24</v>
       </c>
       <c r="G69" t="n">
-        <v>235</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>B0C1ZZ57ZW</t>
+          <t>B0CH92B3S2</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>A620M GAMING X</t>
+          <t>B650M D3HP</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>4.42</v>
+        <v>280.8</v>
       </c>
       <c r="D70" t="n">
-        <v>17</v>
+        <v>216</v>
       </c>
       <c r="E70" t="n">
-        <v>12</v>
+        <v>256</v>
       </c>
       <c r="F70" t="n">
-        <v>24</v>
+        <v>296</v>
       </c>
       <c r="G70" t="n">
-        <v>49</v>
+        <v>358</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>B0CH92B3S2</t>
+          <t>B083RW9KDM</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>B650M D3HP</t>
+          <t>Z790 A ELITE X WIFI7</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>280.8</v>
+        <v>144.3</v>
       </c>
       <c r="D71" t="n">
-        <v>216</v>
+        <v>111</v>
       </c>
       <c r="E71" t="n">
-        <v>256</v>
+        <v>133</v>
       </c>
       <c r="F71" t="n">
-        <v>296</v>
+        <v>156</v>
       </c>
       <c r="G71" t="n">
-        <v>358</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>B083RW9KDM</t>
+          <t>B083RW9TJF</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Z790 A ELITE X WIFI7</t>
+          <t>Z790 AORUS PRO X</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>144.3</v>
+        <v>167.7</v>
       </c>
       <c r="D72" t="n">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="E72" t="n">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="F72" t="n">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="G72" t="n">
-        <v>194</v>
+        <v>216</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>B083RW9TJF</t>
+          <t>B083RVN2VG</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Z790 AORUS PRO X</t>
+          <t>A620I AX</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>167.7</v>
+        <v>325</v>
       </c>
       <c r="D73" t="n">
-        <v>129</v>
+        <v>250</v>
       </c>
       <c r="E73" t="n">
-        <v>153</v>
+        <v>302</v>
       </c>
       <c r="F73" t="n">
-        <v>178</v>
+        <v>356</v>
       </c>
       <c r="G73" t="n">
-        <v>216</v>
+        <v>443</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>B083RVN2VG</t>
+          <t>B0CNR8Y29S</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>A620I AX</t>
+          <t>X670 GAMING X AX V2</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>325</v>
+        <v>236.6</v>
       </c>
       <c r="D74" t="n">
-        <v>250</v>
+        <v>182</v>
       </c>
       <c r="E74" t="n">
-        <v>302</v>
+        <v>218</v>
       </c>
       <c r="F74" t="n">
-        <v>356</v>
+        <v>253</v>
       </c>
       <c r="G74" t="n">
-        <v>443</v>
+        <v>305</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>B0CNR8Y29S</t>
+          <t>B0CN76TH9S</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>X670 GAMING X AX V2</t>
+          <t>X670E AORUS PRO X</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>236.6</v>
+        <v>46.86</v>
       </c>
       <c r="D75" t="n">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E75" t="n">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="F75" t="n">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="G75" t="n">
-        <v>305</v>
+        <v>396</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>B0CN76TH9S</t>
+          <t>B0CKS6BMH7</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>X670E AORUS PRO X</t>
+          <t>Z790 A ELITE AX ICE</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>46.86</v>
+        <v>116</v>
       </c>
       <c r="D76" t="n">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="E76" t="n">
-        <v>206</v>
+        <v>147</v>
       </c>
       <c r="F76" t="n">
-        <v>277</v>
+        <v>176</v>
       </c>
       <c r="G76" t="n">
-        <v>396</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>B0CKS6BMH7</t>
+          <t>B083RVX2FQ</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Z790 A ELITE AX ICE</t>
+          <t>Z790 AORUS MASTER X</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D77" t="n">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="E77" t="n">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="F77" t="n">
-        <v>176</v>
+        <v>111</v>
       </c>
       <c r="G77" t="n">
-        <v>222</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>B083RVX2FQ</t>
+          <t>B0CMJSH15D</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Z790 AORUS MASTER X</t>
+          <t>B650 A ELITE AX ICE</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>104</v>
+        <v>1084.2</v>
       </c>
       <c r="D78" t="n">
-        <v>80</v>
+        <v>834</v>
       </c>
       <c r="E78" t="n">
-        <v>96</v>
+        <v>972</v>
       </c>
       <c r="F78" t="n">
-        <v>111</v>
+        <v>1093</v>
       </c>
       <c r="G78" t="n">
-        <v>137</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>B0CMJSH15D</t>
+          <t>B0CCWLMK56</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>B650 A ELITE AX ICE</t>
+          <t xml:space="preserve">B650M C V2                    </t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1084.2</v>
+        <v>8.32</v>
       </c>
       <c r="D79" t="n">
-        <v>834</v>
+        <v>12</v>
       </c>
       <c r="E79" t="n">
-        <v>972</v>
+        <v>16</v>
       </c>
       <c r="F79" t="n">
-        <v>1093</v>
+        <v>20</v>
       </c>
       <c r="G79" t="n">
-        <v>1278</v>
+        <v>28</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>B09SVZRM13</t>
+          <t>B0CMK1W2YX</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t xml:space="preserve">B660 GAMING X AX DDR4         </t>
+          <t xml:space="preserve">B650 A ELITE AX V2            </t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>464.1</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>357</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>421</v>
       </c>
       <c r="F80" t="n">
-        <v>2</v>
+        <v>480</v>
       </c>
       <c r="G80" t="n">
-        <v>3</v>
+        <v>570</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>B0CCWLMK56</t>
+          <t>B0CNR6L1DH</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t xml:space="preserve">B650M C V2                    </t>
+          <t xml:space="preserve">B760M D3H                     </t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>8.32</v>
+        <v>86.26000000000001</v>
       </c>
       <c r="D81" t="n">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="E81" t="n">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="F81" t="n">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="G81" t="n">
-        <v>28</v>
+        <v>177</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>B0CMK1W2YX</t>
+          <t>B0D2V2FPS7</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t xml:space="preserve">B650 A ELITE AX V2            </t>
+          <t>A620M GAMING X AX</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>464.1</v>
+        <v>75.40000000000001</v>
       </c>
       <c r="D82" t="n">
-        <v>357</v>
+        <v>58</v>
       </c>
       <c r="E82" t="n">
-        <v>421</v>
+        <v>73</v>
       </c>
       <c r="F82" t="n">
-        <v>480</v>
+        <v>86</v>
       </c>
       <c r="G82" t="n">
-        <v>570</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>B0CNR6L1DH</t>
+          <t>B0D8WH9NG3</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t xml:space="preserve">B760M D3H                     </t>
+          <t>B550 AORUS ELITE AX V3</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>86.26000000000001</v>
+        <v>172.1</v>
       </c>
       <c r="D83" t="n">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="E83" t="n">
-        <v>123</v>
+        <v>214</v>
       </c>
       <c r="F83" t="n">
-        <v>144</v>
+        <v>250</v>
       </c>
       <c r="G83" t="n">
-        <v>177</v>
+        <v>306</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>B0D2V2FPS7</t>
+          <t>B083TZ68H1</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>A620M GAMING X AX</t>
+          <t>B650 EAGLE AX</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>75.40000000000001</v>
+        <v>3646.5</v>
       </c>
       <c r="D84" t="n">
-        <v>58</v>
+        <v>3129</v>
       </c>
       <c r="E84" t="n">
-        <v>73</v>
+        <v>3656</v>
       </c>
       <c r="F84" t="n">
-        <v>86</v>
+        <v>4132</v>
       </c>
       <c r="G84" t="n">
-        <v>107</v>
+        <v>4858</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>B0D8WH9NG3</t>
+          <t>B0CTTY491F</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>B550 AORUS ELITE AX V3</t>
+          <t>B650 GAMING X AX V2</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>172.1</v>
+        <v>39</v>
       </c>
       <c r="D85" t="n">
-        <v>179</v>
+        <v>69</v>
       </c>
       <c r="E85" t="n">
-        <v>214</v>
+        <v>80</v>
       </c>
       <c r="F85" t="n">
-        <v>250</v>
+        <v>114</v>
       </c>
       <c r="G85" t="n">
-        <v>306</v>
+        <v>176</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>B083TZ68H1</t>
+          <t>B0CTNYTX8Y</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>B650 EAGLE AX</t>
+          <t>B650 UD AC</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>3646.5</v>
+        <v>14.68</v>
       </c>
       <c r="D86" t="n">
-        <v>3129</v>
+        <v>18</v>
       </c>
       <c r="E86" t="n">
-        <v>3656</v>
+        <v>24</v>
       </c>
       <c r="F86" t="n">
-        <v>4132</v>
+        <v>28</v>
       </c>
       <c r="G86" t="n">
-        <v>4858</v>
+        <v>37</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>B0CTTY491F</t>
+          <t>B0DFHPZBGM</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>B650 GAMING X AX V2</t>
+          <t>B650 UD AX</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>39</v>
+        <v>15.6</v>
       </c>
       <c r="D87" t="n">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="E87" t="n">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="F87" t="n">
-        <v>114</v>
+        <v>19</v>
       </c>
       <c r="G87" t="n">
-        <v>176</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>B0CTNYTX8Y</t>
+          <t>B0CTNXBRJV</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>B650 UD AC</t>
+          <t>B650E AORUS Elite X AX ICE</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>14.68</v>
+        <v>163.8</v>
       </c>
       <c r="D88" t="n">
-        <v>18</v>
+        <v>162</v>
       </c>
       <c r="E88" t="n">
-        <v>24</v>
+        <v>193</v>
       </c>
       <c r="F88" t="n">
-        <v>28</v>
+        <v>224</v>
       </c>
       <c r="G88" t="n">
-        <v>37</v>
+        <v>271</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>B0DFHPZBGM</t>
+          <t>B083SJLWL9</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>B650 UD AX</t>
+          <t>B650M AORUS ELITE AX ICE</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>15.6</v>
+        <v>318.2</v>
       </c>
       <c r="D89" t="n">
-        <v>12</v>
+        <v>320</v>
       </c>
       <c r="E89" t="n">
-        <v>15</v>
+        <v>368</v>
       </c>
       <c r="F89" t="n">
-        <v>19</v>
+        <v>413</v>
       </c>
       <c r="G89" t="n">
-        <v>26</v>
+        <v>478</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>B0CTNXBRJV</t>
+          <t>B0D8WKK29M</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>B650E AORUS Elite X AX ICE</t>
+          <t>B650M C V3</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>163.8</v>
+        <v>3.44</v>
       </c>
       <c r="D90" t="n">
-        <v>162</v>
+        <v>4</v>
       </c>
       <c r="E90" t="n">
-        <v>193</v>
+        <v>4</v>
       </c>
       <c r="F90" t="n">
-        <v>224</v>
+        <v>8</v>
       </c>
       <c r="G90" t="n">
-        <v>271</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>B083SJLWL9</t>
+          <t>B0CTTXH95Q</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>B650M AORUS ELITE AX ICE</t>
+          <t>B650M D3HP AX</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>318.2</v>
+        <v>43.08</v>
       </c>
       <c r="D91" t="n">
-        <v>320</v>
+        <v>58</v>
       </c>
       <c r="E91" t="n">
-        <v>368</v>
+        <v>61</v>
       </c>
       <c r="F91" t="n">
-        <v>413</v>
+        <v>97</v>
       </c>
       <c r="G91" t="n">
-        <v>478</v>
+        <v>168</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>B0D8WKK29M</t>
+          <t>B0D2V4VH2C</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>B650M C V3</t>
+          <t>B650M GAMING PLUS WIFI</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>3.44</v>
+        <v>514.3</v>
       </c>
       <c r="D92" t="n">
-        <v>4</v>
+        <v>613</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>722</v>
       </c>
       <c r="F92" t="n">
-        <v>8</v>
+        <v>827</v>
       </c>
       <c r="G92" t="n">
-        <v>12</v>
+        <v>985</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>B0CTTXH95Q</t>
+          <t>B0CTTW2MVG</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>B650M D3HP AX</t>
+          <t>B760 DS3H AC</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>43.08</v>
+        <v>7.46</v>
       </c>
       <c r="D93" t="n">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="E93" t="n">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="F93" t="n">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="G93" t="n">
-        <v>168</v>
+        <v>29</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>B0D2V4VH2C</t>
+          <t>B0CTTWZCVK</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>B650M GAMING PLUS WIFI</t>
+          <t>B760 DS3H AX</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>514.3</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="D94" t="n">
-        <v>613</v>
+        <v>12</v>
       </c>
       <c r="E94" t="n">
-        <v>722</v>
+        <v>16</v>
       </c>
       <c r="F94" t="n">
-        <v>827</v>
+        <v>20</v>
       </c>
       <c r="G94" t="n">
-        <v>985</v>
+        <v>27</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>B0CTTW2MVG</t>
+          <t>B0D54QJ9CJ</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>B760 DS3H AC</t>
+          <t>B760M GAMING PLUS WIFI DDR4</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7.46</v>
+        <v>330.6</v>
       </c>
       <c r="D95" t="n">
-        <v>12</v>
+        <v>390</v>
       </c>
       <c r="E95" t="n">
-        <v>16</v>
+        <v>453</v>
       </c>
       <c r="F95" t="n">
-        <v>21</v>
+        <v>507</v>
       </c>
       <c r="G95" t="n">
-        <v>29</v>
+        <v>592</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>B0CTTWZCVK</t>
+          <t>B0D33M6CB7</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>B760 DS3H AX</t>
+          <t>GC-WIFI7</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8.800000000000001</v>
+        <v>189.8</v>
       </c>
       <c r="D96" t="n">
-        <v>12</v>
+        <v>164</v>
       </c>
       <c r="E96" t="n">
-        <v>16</v>
+        <v>194</v>
       </c>
       <c r="F96" t="n">
-        <v>20</v>
+        <v>222</v>
       </c>
       <c r="G96" t="n">
-        <v>27</v>
+        <v>265</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>B0D54QJ9CJ</t>
+          <t>B0CPW1F841</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>B760M GAMING PLUS WIFI DDR4</t>
+          <t>TRX50 AERO D</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>330.6</v>
+        <v>53.84</v>
       </c>
       <c r="D97" t="n">
-        <v>390</v>
+        <v>84</v>
       </c>
       <c r="E97" t="n">
-        <v>453</v>
+        <v>100</v>
       </c>
       <c r="F97" t="n">
-        <v>507</v>
+        <v>114</v>
       </c>
       <c r="G97" t="n">
-        <v>592</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>B0D33M6CB7</t>
+          <t>B0DGVC3DDW</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>GC-WIFI7</t>
+          <t>X870 AORUS ELITE WIFI7</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>213.2</v>
+        <v>1141.126</v>
       </c>
       <c r="D98" t="n">
-        <v>164</v>
+        <v>1694</v>
       </c>
       <c r="E98" t="n">
-        <v>194</v>
+        <v>2004</v>
       </c>
       <c r="F98" t="n">
-        <v>222</v>
+        <v>2304</v>
       </c>
       <c r="G98" t="n">
-        <v>265</v>
+        <v>2769</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>B0CPW1F841</t>
+          <t>B0DGVGRVLQ</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>TRX50 AERO D</t>
+          <t>X870 AORUS ELITE WIFI7 ICE</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>53.84</v>
+        <v>857.182</v>
       </c>
       <c r="D99" t="n">
-        <v>84</v>
+        <v>1220</v>
       </c>
       <c r="E99" t="n">
-        <v>100</v>
+        <v>1409</v>
       </c>
       <c r="F99" t="n">
-        <v>114</v>
+        <v>1572</v>
       </c>
       <c r="G99" t="n">
-        <v>137</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>B0DGVC3DDW</t>
+          <t>B0DGVMYTW6</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>X870 AORUS ELITE WIFI7</t>
+          <t>X870 EAGLE WIFI7</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>1184</v>
+        <v>1237.6</v>
       </c>
       <c r="D100" t="n">
-        <v>1694</v>
+        <v>952</v>
       </c>
       <c r="E100" t="n">
-        <v>2004</v>
+        <v>1124</v>
       </c>
       <c r="F100" t="n">
-        <v>2304</v>
+        <v>1289</v>
       </c>
       <c r="G100" t="n">
-        <v>2769</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>B0DGVGRVLQ</t>
+          <t>B0DHWLN5XT</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>X870 AORUS ELITE WIFI7 ICE</t>
+          <t>X870 GAMING WIFI6</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>758.2</v>
+        <v>424.87</v>
       </c>
       <c r="D101" t="n">
-        <v>1220</v>
+        <v>342</v>
       </c>
       <c r="E101" t="n">
-        <v>1409</v>
+        <v>404</v>
       </c>
       <c r="F101" t="n">
-        <v>1572</v>
+        <v>463</v>
       </c>
       <c r="G101" t="n">
-        <v>1818</v>
+        <v>553</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>B0DGVMYTW6</t>
+          <t>B0DGVGT3PJ</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>X870 EAGLE WIFI7</t>
+          <t>X870 GAMING X WIFI7</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>980.8000000000001</v>
+        <v>381.4760000000001</v>
       </c>
       <c r="D102" t="n">
-        <v>952</v>
+        <v>499</v>
       </c>
       <c r="E102" t="n">
-        <v>1124</v>
+        <v>589</v>
       </c>
       <c r="F102" t="n">
-        <v>1289</v>
+        <v>674</v>
       </c>
       <c r="G102" t="n">
-        <v>1543</v>
+        <v>805</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>B0DHWLN5XT</t>
+          <t>B0DGVBM73J</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>X870 GAMING WIFI6</t>
+          <t>X870E AORUS ELITE WIFI7</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>444.6</v>
+        <v>651.558</v>
       </c>
       <c r="D103" t="n">
-        <v>342</v>
+        <v>900</v>
       </c>
       <c r="E103" t="n">
-        <v>404</v>
+        <v>1047</v>
       </c>
       <c r="F103" t="n">
-        <v>463</v>
+        <v>1179</v>
       </c>
       <c r="G103" t="n">
-        <v>553</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>B0DGVGT3PJ</t>
+          <t>B0DGVSW4FD</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>X870 GAMING X WIFI7</t>
+          <t>X870E AORUS MASTER</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>466.6</v>
+        <v>271.91</v>
       </c>
       <c r="D104" t="n">
-        <v>499</v>
+        <v>213</v>
       </c>
       <c r="E104" t="n">
-        <v>589</v>
+        <v>253</v>
       </c>
       <c r="F104" t="n">
-        <v>674</v>
+        <v>290</v>
       </c>
       <c r="G104" t="n">
-        <v>805</v>
+        <v>348</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>B0DGVBM73J</t>
+          <t>B0DGVGV7YN</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>X870E AORUS ELITE WIFI7</t>
+          <t>X870E AORUS PRO</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>626.4000000000001</v>
+        <v>228.46</v>
       </c>
       <c r="D105" t="n">
-        <v>900</v>
+        <v>246</v>
       </c>
       <c r="E105" t="n">
-        <v>1047</v>
+        <v>288</v>
       </c>
       <c r="F105" t="n">
-        <v>1179</v>
+        <v>324</v>
       </c>
       <c r="G105" t="n">
-        <v>1382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>B0DGVSW4FD</t>
+          <t>B0DGVBSLLP</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>X870E AORUS MASTER</t>
+          <t>X870E AORUS PRO ICE</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>276.9</v>
+        <v>627.3</v>
       </c>
       <c r="D106" t="n">
-        <v>213</v>
+        <v>723</v>
       </c>
       <c r="E106" t="n">
-        <v>253</v>
+        <v>823</v>
       </c>
       <c r="F106" t="n">
-        <v>290</v>
+        <v>903</v>
       </c>
       <c r="G106" t="n">
-        <v>348</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>B0DGVGV7YN</t>
+          <t>B0CTTVFWHM</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>X870E AORUS PRO</t>
+          <t>Z790 AORUS PRO X WIFI7</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>319.8</v>
+        <v>115.6</v>
       </c>
       <c r="D107" t="n">
-        <v>246</v>
+        <v>111</v>
       </c>
       <c r="E107" t="n">
-        <v>288</v>
+        <v>133</v>
       </c>
       <c r="F107" t="n">
-        <v>324</v>
+        <v>155</v>
       </c>
       <c r="G107" t="n">
-        <v>380</v>
+        <v>189</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>B0DGVBSLLP</t>
+          <t>B0CTTWH6TD</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>X870E AORUS PRO ICE</t>
+          <t>Z790 D AC</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>939.9</v>
+        <v>15.42</v>
       </c>
       <c r="D108" t="n">
-        <v>723</v>
+        <v>17</v>
       </c>
       <c r="E108" t="n">
-        <v>823</v>
+        <v>22</v>
       </c>
       <c r="F108" t="n">
-        <v>903</v>
+        <v>29</v>
       </c>
       <c r="G108" t="n">
-        <v>1024</v>
+        <v>37</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>B0CTTVFWHM</t>
+          <t>B0CTNPZLNH</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Z790 AORUS PRO X WIFI7</t>
+          <t>Z790 Eagle AX</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>115.6</v>
+        <v>232.6</v>
       </c>
       <c r="D109" t="n">
-        <v>111</v>
+        <v>194</v>
       </c>
       <c r="E109" t="n">
-        <v>133</v>
+        <v>236</v>
       </c>
       <c r="F109" t="n">
-        <v>155</v>
+        <v>279</v>
       </c>
       <c r="G109" t="n">
-        <v>189</v>
+        <v>349</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>B0CTTWH6TD</t>
+          <t>B0D8WH39QJ</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Z790 D AC</t>
+          <t>Z790 GAMING PLUS AX</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>15.42</v>
+        <v>58.9</v>
       </c>
       <c r="D110" t="n">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E110" t="n">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="F110" t="n">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="G110" t="n">
-        <v>37</v>
+        <v>140</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>B0CTNPZLNH</t>
+          <t>B0D2RL4PT6</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Z790 Eagle AX</t>
+          <t>Z790 S WIFI DDR4</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>240.6</v>
+        <v>557</v>
       </c>
       <c r="D111" t="n">
-        <v>194</v>
+        <v>467</v>
       </c>
       <c r="E111" t="n">
-        <v>236</v>
+        <v>552</v>
       </c>
       <c r="F111" t="n">
-        <v>279</v>
+        <v>636</v>
       </c>
       <c r="G111" t="n">
-        <v>349</v>
+        <v>767</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>B0D8WH39QJ</t>
+          <t>B0D2PK3CC1</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Z790 GAMING PLUS AX</t>
+          <t>Z790M AORUS ELITE AX ICE</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>58.9</v>
+        <v>179.4</v>
       </c>
       <c r="D112" t="n">
-        <v>49</v>
+        <v>180</v>
       </c>
       <c r="E112" t="n">
-        <v>50</v>
+        <v>212</v>
       </c>
       <c r="F112" t="n">
-        <v>81</v>
+        <v>242</v>
       </c>
       <c r="G112" t="n">
-        <v>140</v>
+        <v>289</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>B0D2RL4PT6</t>
+          <t>B0DJP9KLLD</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Z790 S WIFI DDR4</t>
+          <t>Z890 AERO G</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>464.5</v>
+        <v>29.65</v>
       </c>
       <c r="D113" t="n">
-        <v>467</v>
+        <v>37</v>
       </c>
       <c r="E113" t="n">
-        <v>552</v>
+        <v>45</v>
       </c>
       <c r="F113" t="n">
-        <v>636</v>
+        <v>56</v>
       </c>
       <c r="G113" t="n">
-        <v>767</v>
+        <v>73</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>B0D2PK3CC1</t>
+          <t>B0DJP95MGB</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Z790M AORUS ELITE AX ICE</t>
+          <t>Z890 AORUS ELITE WIFI7</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>179.4</v>
+        <v>164.03</v>
       </c>
       <c r="D114" t="n">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="E114" t="n">
-        <v>212</v>
+        <v>170</v>
       </c>
       <c r="F114" t="n">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="G114" t="n">
-        <v>289</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>B0DJP9KLLD</t>
+          <t>B0DJP7NRXX</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Z890 AERO G</t>
+          <t>Z890 AORUS ELITE WIFI7 ICE</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>22.87</v>
+        <v>74.10000000000001</v>
       </c>
       <c r="D115" t="n">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="E115" t="n">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F115" t="n">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="G115" t="n">
-        <v>73</v>
+        <v>107</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>B0DJP95MGB</t>
+          <t>B0DJP76L1F</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Z890 AORUS ELITE WIFI7</t>
+          <t>Z890 AORUS ELITE X ICE</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>124.78</v>
+        <v>11.712</v>
       </c>
       <c r="D116" t="n">
-        <v>142</v>
+        <v>20</v>
       </c>
       <c r="E116" t="n">
-        <v>170</v>
+        <v>26</v>
       </c>
       <c r="F116" t="n">
-        <v>197</v>
+        <v>33</v>
       </c>
       <c r="G116" t="n">
-        <v>241</v>
+        <v>45</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>B0DJP7NRXX</t>
+          <t>B0DJP9LCYC</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Z890 AORUS ELITE WIFI7 ICE</t>
+          <t>Z890 AORUS MASTER</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>74.10000000000001</v>
+        <v>23.368</v>
       </c>
       <c r="D117" t="n">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="E117" t="n">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="F117" t="n">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="G117" t="n">
-        <v>107</v>
+        <v>68</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>B0DJP76L1F</t>
+          <t>B0DJP8NFWP</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Z890 AORUS ELITE X ICE</t>
+          <t>Z890 AORUS PRO ICE</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>11.48</v>
+        <v>37.398</v>
       </c>
       <c r="D118" t="n">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="E118" t="n">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="F118" t="n">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="G118" t="n">
-        <v>45</v>
+        <v>144</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>B0DJP9LCYC</t>
+          <t>B0DJP8MMMJ</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Z890 AORUS MASTER</t>
+          <t>Z890 EAGLE WIFI7</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>22.22</v>
+        <v>38.188</v>
       </c>
       <c r="D119" t="n">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E119" t="n">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="F119" t="n">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="G119" t="n">
-        <v>68</v>
+        <v>108</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>B0DJP8NFWP</t>
+          <t>B0DJP9DBVS</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Z890 AORUS PRO ICE</t>
+          <t>Z890 GAMING X WIFI7</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>38.32000000000001</v>
+        <v>14.79</v>
       </c>
       <c r="D120" t="n">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="E120" t="n">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="F120" t="n">
-        <v>109</v>
+        <v>26</v>
       </c>
       <c r="G120" t="n">
-        <v>144</v>
+        <v>35</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>B0DJP8MMMJ</t>
+          <t>B0DJP8W3BY</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Z890 EAGLE WIFI7</t>
+          <t>Z890 UD WIFI6E</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>37.90000000000001</v>
+        <v>50.688</v>
       </c>
       <c r="D121" t="n">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="E121" t="n">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="F121" t="n">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="G121" t="n">
-        <v>108</v>
+        <v>162</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>B0DJP9DBVS</t>
+          <t>B0DJP82ML2</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Z890 GAMING X WIFI7</t>
+          <t>Z890I AORUS ULTRA</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>14.56</v>
+        <v>27.36</v>
       </c>
       <c r="D122" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E122" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F122" t="n">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="G122" t="n">
-        <v>35</v>
+        <v>71</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>B0DJP8W3BY</t>
+          <t>B0DJP8Q6JK</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Z890 UD WIFI6E</t>
+          <t>Z890M AORUS ELITE WIFI7 ICE</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>49.6</v>
+        <v>47.03</v>
       </c>
       <c r="D123" t="n">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="E123" t="n">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="F123" t="n">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="G123" t="n">
-        <v>162</v>
+        <v>128</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>B0DJP82ML2</t>
+          <t>B0DJP9FZYK</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Z890I AORUS ULTRA</t>
+          <t>Z890M GAMING X</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>27.36</v>
+        <v>34.73999999999999</v>
       </c>
       <c r="D124" t="n">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="E124" t="n">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="F124" t="n">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="G124" t="n">
-        <v>71</v>
+        <v>142</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>B0DJP8Q6JK</t>
+          <t>B081JDLX48</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Z890M AORUS ELITE WIFI7 ICE</t>
+          <t>TRX40 AORUS MASTER</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>45.58</v>
+        <v>4</v>
       </c>
       <c r="D125" t="n">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="E125" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="G125" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>B0DJP9FZYK</t>
+          <t>B0DQLJVH25</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Z890M GAMING X</t>
+          <t>B850 AI TOP</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>43.26000000000001</v>
+        <v>13</v>
       </c>
       <c r="D126" t="n">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="E126" t="n">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="F126" t="n">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="G126" t="n">
-        <v>142</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>B081JDLX48</t>
+          <t>B0DQLHVQSF</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>TRX40 AORUS MASTER</t>
+          <t>B850 AORUS ELITE WIFI7</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>4</v>
+        <v>106</v>
       </c>
       <c r="D127" t="n">
-        <v>4</v>
-      </c>
-      <c r="E127" t="inlineStr"/>
-      <c r="F127" t="inlineStr"/>
-      <c r="G127" t="inlineStr"/>
+        <v>115</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
+      <c r="F127" t="n">
+        <v>0</v>
+      </c>
+      <c r="G127" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>B0DQLJVH25</t>
+          <t>B0DQLKRXKW</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>B850 AI TOP</t>
+          <t>B850 AORUS ELITE WIFI7 ICE</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>13</v>
+        <v>176</v>
       </c>
       <c r="D128" t="n">
-        <v>13</v>
-      </c>
-      <c r="E128" t="inlineStr"/>
-      <c r="F128" t="inlineStr"/>
-      <c r="G128" t="inlineStr"/>
+        <v>195</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
+      <c r="F128" t="n">
+        <v>0</v>
+      </c>
+      <c r="G128" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>B0DQLHVQSF</t>
+          <t>B0DQLJWRDX</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>B850 AORUS ELITE WIFI7</t>
+          <t>B850 EAGLE WIFI6E</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="D129" t="n">
-        <v>115</v>
-      </c>
-      <c r="E129" t="inlineStr"/>
-      <c r="F129" t="inlineStr"/>
-      <c r="G129" t="inlineStr"/>
+        <v>133</v>
+      </c>
+      <c r="E129" t="n">
+        <v>0</v>
+      </c>
+      <c r="F129" t="n">
+        <v>0</v>
+      </c>
+      <c r="G129" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>B0DQLKRXKW</t>
+          <t>B0DQLKZSKF</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>B850 AORUS ELITE WIFI7 ICE</t>
+          <t>B850 GAMING WIFI6</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>176</v>
+        <v>15</v>
       </c>
       <c r="D130" t="n">
-        <v>195</v>
-      </c>
-      <c r="E130" t="inlineStr"/>
-      <c r="F130" t="inlineStr"/>
-      <c r="G130" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0</v>
+      </c>
+      <c r="F130" t="n">
+        <v>0</v>
+      </c>
+      <c r="G130" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>B0DQLJWRDX</t>
+          <t>B0DQLH22F6</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>B850 EAGLE WIFI6E</t>
+          <t>B850 GAMING X WIFI6E</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="D131" t="n">
-        <v>133</v>
-      </c>
-      <c r="E131" t="inlineStr"/>
-      <c r="F131" t="inlineStr"/>
-      <c r="G131" t="inlineStr"/>
+        <v>14</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
+      <c r="F131" t="n">
+        <v>0</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>B0DQLKZSKF</t>
+          <t>B0DQLKPSMG</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>B850 GAMING WIFI6</t>
+          <t>B850I AORUS PRO</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="D132" t="n">
-        <v>16</v>
-      </c>
-      <c r="E132" t="inlineStr"/>
-      <c r="F132" t="inlineStr"/>
-      <c r="G132" t="inlineStr"/>
+        <v>112</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+      <c r="F132" t="n">
+        <v>0</v>
+      </c>
+      <c r="G132" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>B0DQLH22F6</t>
+          <t>B0DQLJGTRM</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>B850 GAMING X WIFI6E</t>
+          <t>B850M AORUS ELITE WIFI6E ICE</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>13</v>
+        <v>279</v>
       </c>
       <c r="D133" t="n">
-        <v>14</v>
-      </c>
-      <c r="E133" t="inlineStr"/>
-      <c r="F133" t="inlineStr"/>
-      <c r="G133" t="inlineStr"/>
+        <v>310</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0</v>
+      </c>
+      <c r="F133" t="n">
+        <v>0</v>
+      </c>
+      <c r="G133" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>B0DQLKPSMG</t>
+          <t>B0DQLJHJ8B</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>B850I AORUS PRO</t>
+          <t>B850M DS3H</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="D134" t="n">
-        <v>112</v>
-      </c>
-      <c r="E134" t="inlineStr"/>
-      <c r="F134" t="inlineStr"/>
-      <c r="G134" t="inlineStr"/>
+        <v>43</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
+      <c r="F134" t="n">
+        <v>0</v>
+      </c>
+      <c r="G134" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>B0DQLJGTRM</t>
+          <t>B0DQLHLVLK</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>B850M AORUS ELITE WIFI6E ICE</t>
+          <t>B850M GAMING X WIFI6E</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>279</v>
+        <v>107</v>
       </c>
       <c r="D135" t="n">
-        <v>310</v>
-      </c>
-      <c r="E135" t="inlineStr"/>
-      <c r="F135" t="inlineStr"/>
-      <c r="G135" t="inlineStr"/>
+        <v>119</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0</v>
+      </c>
+      <c r="F135" t="n">
+        <v>0</v>
+      </c>
+      <c r="G135" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>B0DQLJHJ8B</t>
+          <t>B0DQLH4ZTR</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>B850M DS3H</t>
+          <t>B860 AORUS ELITE WIFI7 ICE</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="D136" t="n">
-        <v>43</v>
-      </c>
-      <c r="E136" t="inlineStr"/>
-      <c r="F136" t="inlineStr"/>
-      <c r="G136" t="inlineStr"/>
+        <v>9</v>
+      </c>
+      <c r="E136" t="n">
+        <v>0</v>
+      </c>
+      <c r="F136" t="n">
+        <v>0</v>
+      </c>
+      <c r="G136" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>B0DQLHLVLK</t>
+          <t>B0DQLJRY8C</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>B850M GAMING X WIFI6E</t>
+          <t>B860 EAGLE WIFI6E</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>107</v>
+        <v>10</v>
       </c>
       <c r="D137" t="n">
-        <v>119</v>
-      </c>
-      <c r="E137" t="inlineStr"/>
-      <c r="F137" t="inlineStr"/>
-      <c r="G137" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="E137" t="n">
+        <v>0</v>
+      </c>
+      <c r="F137" t="n">
+        <v>0</v>
+      </c>
+      <c r="G137" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>B0DQLH4ZTR</t>
+          <t>B0DQLLLHYY</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>B860 AORUS ELITE WIFI7 ICE</t>
+          <t>B860 GAMING X WIFI6E</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D138" t="n">
-        <v>9</v>
-      </c>
-      <c r="E138" t="inlineStr"/>
-      <c r="F138" t="inlineStr"/>
-      <c r="G138" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="E138" t="n">
+        <v>0</v>
+      </c>
+      <c r="F138" t="n">
+        <v>0</v>
+      </c>
+      <c r="G138" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>B0DQLJRY8C</t>
+          <t>B0DQLGMGVP</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>B860 EAGLE WIFI6E</t>
+          <t>B860M AORUS ELITE WIFI6E ICE</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D139" t="n">
-        <v>10</v>
-      </c>
-      <c r="E139" t="inlineStr"/>
-      <c r="F139" t="inlineStr"/>
-      <c r="G139" t="inlineStr"/>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>B0DQLLLHYY</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>B860 GAMING X WIFI6E</t>
-        </is>
-      </c>
-      <c r="C140" t="n">
-        <v>10</v>
-      </c>
-      <c r="D140" t="n">
-        <v>11</v>
-      </c>
-      <c r="E140" t="inlineStr"/>
-      <c r="F140" t="inlineStr"/>
-      <c r="G140" t="inlineStr"/>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>B0DQLGMGVP</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>B860M AORUS ELITE WIFI6E ICE</t>
-        </is>
-      </c>
-      <c r="C141" t="n">
         <v>9</v>
       </c>
-      <c r="D141" t="n">
-        <v>9</v>
-      </c>
-      <c r="E141" t="inlineStr"/>
-      <c r="F141" t="inlineStr"/>
-      <c r="G141" t="inlineStr"/>
+      <c r="E139" t="n">
+        <v>0</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0</v>
+      </c>
+      <c r="G139" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed update to excel issue
</commit_message>
<xml_diff>
--- a/4_week_report.xlsx
+++ b/4_week_report.xlsx
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="D9" t="n">
         <v>374</v>
@@ -725,7 +725,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>771.8000000000001</v>
+        <v>780.8000000000001</v>
       </c>
       <c r="D11" t="n">
         <v>651</v>
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2423</v>
+        <v>2408</v>
       </c>
       <c r="D14" t="n">
         <v>2394</v>
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>159</v>
+        <v>166.5</v>
       </c>
       <c r="D15" t="n">
         <v>143</v>
@@ -995,7 +995,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="D21" t="n">
         <v>407</v>
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1073.9</v>
+        <v>1065.9</v>
       </c>
       <c r="D26" t="n">
         <v>934</v>
@@ -1238,7 +1238,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>91.00000000000001</v>
+        <v>57.00000000000001</v>
       </c>
       <c r="D30" t="n">
         <v>70</v>
@@ -1346,7 +1346,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>12.88</v>
+        <v>12.78</v>
       </c>
       <c r="D34" t="n">
         <v>48</v>
@@ -1454,7 +1454,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>49.2</v>
+        <v>40</v>
       </c>
       <c r="D38" t="n">
         <v>54</v>
@@ -1751,7 +1751,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>57.36</v>
+        <v>58.16000000000001</v>
       </c>
       <c r="D49" t="n">
         <v>186</v>
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D52" t="n">
         <v>206</v>
@@ -2480,7 +2480,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D76" t="n">
         <v>121</v>

</xml_diff>

<commit_message>
added 4wk low sales check
</commit_message>
<xml_diff>
--- a/4_week_report.xlsx
+++ b/4_week_report.xlsx
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2.58</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
         <v>10</v>
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>204</v>
+        <v>212.6</v>
       </c>
       <c r="D3" t="n">
         <v>313</v>
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4.600000000000001</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
         <v>4</v>
@@ -563,7 +563,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3.28</v>
+        <v>2.6</v>
       </c>
       <c r="D5" t="n">
         <v>10</v>
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.44</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
         <v>4</v>
@@ -644,7 +644,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>322.3000000000001</v>
+        <v>516</v>
       </c>
       <c r="D8" t="n">
         <v>251</v>
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>501.8</v>
+        <v>569</v>
       </c>
       <c r="D9" t="n">
         <v>386</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>27.3</v>
+        <v>36</v>
       </c>
       <c r="D10" t="n">
         <v>21</v>
@@ -725,7 +725,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>361.4</v>
+        <v>527</v>
       </c>
       <c r="D11" t="n">
         <v>278</v>
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2.92</v>
+        <v>3.800000000000001</v>
       </c>
       <c r="D12" t="n">
         <v>8</v>
@@ -779,7 +779,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>5.28</v>
+        <v>6.4</v>
       </c>
       <c r="D13" t="n">
         <v>8</v>
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2587</v>
+        <v>2542</v>
       </c>
       <c r="D14" t="n">
         <v>2456</v>
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>129.5</v>
+        <v>140</v>
       </c>
       <c r="D15" t="n">
         <v>101</v>
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4.12</v>
+        <v>1.6</v>
       </c>
       <c r="D16" t="n">
         <v>17</v>
@@ -914,7 +914,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>8.040000000000001</v>
+        <v>9.6</v>
       </c>
       <c r="D18" t="n">
         <v>14</v>
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>174.2</v>
+        <v>208</v>
       </c>
       <c r="D19" t="n">
         <v>134</v>
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2.8</v>
+        <v>2</v>
       </c>
       <c r="D20" t="n">
         <v>8</v>
@@ -995,7 +995,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D21" t="n">
         <v>419</v>
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>6.000000000000001</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
         <v>24</v>
@@ -1049,7 +1049,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>292.5</v>
+        <v>250.6</v>
       </c>
       <c r="D23" t="n">
         <v>225</v>
@@ -1103,7 +1103,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.5599999999999999</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
         <v>4</v>
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>753.7</v>
+        <v>800</v>
       </c>
       <c r="D26" t="n">
         <v>615</v>
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1.12</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
         <v>8</v>
@@ -1184,7 +1184,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D28" t="n">
         <v>289</v>
@@ -1211,7 +1211,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>164.36</v>
+        <v>93</v>
       </c>
       <c r="D29" t="n">
         <v>191</v>
@@ -1238,7 +1238,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>27.8</v>
+        <v>34</v>
       </c>
       <c r="D30" t="n">
         <v>70</v>
@@ -1265,7 +1265,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="D31" t="n">
         <v>9</v>
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>624</v>
+        <v>662</v>
       </c>
       <c r="D32" t="n">
         <v>521</v>
@@ -1319,7 +1319,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>373.1</v>
+        <v>545</v>
       </c>
       <c r="D33" t="n">
         <v>287</v>
@@ -1346,7 +1346,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>10.4</v>
+        <v>1.2</v>
       </c>
       <c r="D34" t="n">
         <v>46</v>
@@ -1454,7 +1454,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>50.7</v>
+        <v>53</v>
       </c>
       <c r="D38" t="n">
         <v>39</v>
@@ -1481,7 +1481,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1021</v>
+        <v>1227</v>
       </c>
       <c r="D39" t="n">
         <v>1044</v>
@@ -1508,7 +1508,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.5599999999999999</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
         <v>4</v>
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>15.92</v>
+        <v>3.4</v>
       </c>
       <c r="D41" t="n">
         <v>52</v>
@@ -1589,7 +1589,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>38.64</v>
+        <v>66</v>
       </c>
       <c r="D43" t="n">
         <v>44</v>
@@ -1616,7 +1616,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>21.46</v>
+        <v>22.8</v>
       </c>
       <c r="D44" t="n">
         <v>43</v>
@@ -1643,7 +1643,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>13.42</v>
+        <v>12.6</v>
       </c>
       <c r="D45" t="n">
         <v>33</v>
@@ -1670,7 +1670,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>364.7</v>
+        <v>359</v>
       </c>
       <c r="D46" t="n">
         <v>301</v>
@@ -1697,7 +1697,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D47" t="n">
         <v>5</v>
@@ -1724,7 +1724,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>3.44</v>
+        <v>3.6</v>
       </c>
       <c r="D48" t="n">
         <v>8</v>
@@ -1751,7 +1751,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>21.56</v>
+        <v>4</v>
       </c>
       <c r="D49" t="n">
         <v>102</v>
@@ -1778,7 +1778,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>616.2</v>
+        <v>832</v>
       </c>
       <c r="D50" t="n">
         <v>474</v>
@@ -1805,7 +1805,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>128.7</v>
+        <v>182</v>
       </c>
       <c r="D51" t="n">
         <v>99</v>
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1.18</v>
+        <v>2</v>
       </c>
       <c r="D52" t="n">
         <v>5</v>
@@ -1859,7 +1859,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="D53" t="n">
         <v>110</v>
@@ -1886,7 +1886,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>92.3</v>
+        <v>115</v>
       </c>
       <c r="D54" t="n">
         <v>71</v>
@@ -1913,7 +1913,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2.08</v>
+        <v>0.8</v>
       </c>
       <c r="D55" t="n">
         <v>8</v>
@@ -1940,7 +1940,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>17.28</v>
+        <v>17.2</v>
       </c>
       <c r="D56" t="n">
         <v>24</v>
@@ -1967,7 +1967,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.5599999999999999</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
         <v>4</v>
@@ -1994,7 +1994,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>209.62</v>
+        <v>237.4</v>
       </c>
       <c r="D58" t="n">
         <v>277</v>
@@ -2021,7 +2021,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>67.10000000000001</v>
+        <v>76</v>
       </c>
       <c r="D59" t="n">
         <v>53</v>
@@ -2048,7 +2048,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>44.8</v>
+        <v>57</v>
       </c>
       <c r="D60" t="n">
         <v>36</v>
@@ -2075,7 +2075,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>32.38000000000001</v>
+        <v>0</v>
       </c>
       <c r="D61" t="n">
         <v>57</v>
@@ -2102,7 +2102,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>367.7</v>
+        <v>388</v>
       </c>
       <c r="D62" t="n">
         <v>294</v>
@@ -2129,7 +2129,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>7.4</v>
+        <v>6</v>
       </c>
       <c r="D63" t="n">
         <v>8</v>
@@ -2156,7 +2156,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>43.8</v>
+        <v>57</v>
       </c>
       <c r="D64" t="n">
         <v>64</v>
@@ -2183,7 +2183,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>11.2</v>
+        <v>14.8</v>
       </c>
       <c r="D65" t="n">
         <v>40</v>
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>81.5</v>
+        <v>96</v>
       </c>
       <c r="D66" t="n">
         <v>63</v>
@@ -2237,7 +2237,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>101.2</v>
+        <v>128</v>
       </c>
       <c r="D67" t="n">
         <v>78</v>
@@ -2291,7 +2291,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>279.7</v>
+        <v>218.8</v>
       </c>
       <c r="D69" t="n">
         <v>226</v>
@@ -2318,7 +2318,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D70" t="n">
         <v>95</v>
@@ -2345,7 +2345,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>159.3</v>
+        <v>167</v>
       </c>
       <c r="D71" t="n">
         <v>126</v>
@@ -2372,7 +2372,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D72" t="n">
         <v>288</v>
@@ -2399,7 +2399,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>148.2</v>
+        <v>136</v>
       </c>
       <c r="D73" t="n">
         <v>141</v>
@@ -2426,7 +2426,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>21.76</v>
+        <v>5.200000000000001</v>
       </c>
       <c r="D74" t="n">
         <v>144</v>
@@ -2453,7 +2453,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>52.12</v>
+        <v>53.2</v>
       </c>
       <c r="D75" t="n">
         <v>82</v>
@@ -2480,7 +2480,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="D76" t="n">
         <v>77</v>
@@ -2507,7 +2507,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>575.9000000000001</v>
+        <v>622.5999999999999</v>
       </c>
       <c r="D77" t="n">
         <v>443</v>
@@ -2561,7 +2561,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="D79" t="n">
         <v>290</v>
@@ -2588,7 +2588,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>50.64000000000001</v>
+        <v>55.40000000000001</v>
       </c>
       <c r="D80" t="n">
         <v>60</v>
@@ -2615,7 +2615,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>28.42</v>
+        <v>30.8</v>
       </c>
       <c r="D81" t="n">
         <v>37</v>
@@ -2642,7 +2642,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>333.1</v>
+        <v>340</v>
       </c>
       <c r="D82" t="n">
         <v>263</v>
@@ -2669,7 +2669,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1851</v>
+        <v>1627</v>
       </c>
       <c r="D83" t="n">
         <v>1684</v>
@@ -2696,7 +2696,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>14.54</v>
+        <v>12.8</v>
       </c>
       <c r="D84" t="n">
         <v>75</v>
@@ -2723,7 +2723,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>8.32</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="D85" t="n">
         <v>12</v>
@@ -2750,7 +2750,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>15</v>
+        <v>7.2</v>
       </c>
       <c r="D86" t="n">
         <v>15</v>
@@ -2777,7 +2777,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>202</v>
+        <v>181.6</v>
       </c>
       <c r="D87" t="n">
         <v>165</v>
@@ -2804,7 +2804,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>327.5</v>
+        <v>1089.8</v>
       </c>
       <c r="D88" t="n">
         <v>280</v>
@@ -2831,7 +2831,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="D89" t="n">
         <v>4</v>
@@ -2858,7 +2858,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>27.46</v>
+        <v>28</v>
       </c>
       <c r="D90" t="n">
         <v>97</v>
@@ -2885,7 +2885,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>422.2</v>
+        <v>448</v>
       </c>
       <c r="D91" t="n">
         <v>330</v>
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>8</v>
+        <v>8.4</v>
       </c>
       <c r="D92" t="n">
         <v>8</v>
@@ -2939,7 +2939,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>5.28</v>
+        <v>6</v>
       </c>
       <c r="D93" t="n">
         <v>8</v>
@@ -2966,7 +2966,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>515.6</v>
+        <v>675.4000000000001</v>
       </c>
       <c r="D94" t="n">
         <v>399</v>
@@ -2993,7 +2993,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>189.8</v>
+        <v>186</v>
       </c>
       <c r="D95" t="n">
         <v>146</v>
@@ -3020,7 +3020,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>54.44</v>
+        <v>51</v>
       </c>
       <c r="D96" t="n">
         <v>85</v>
@@ -3047,7 +3047,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1453.4</v>
+        <v>1605.4</v>
       </c>
       <c r="D97" t="n">
         <v>1118</v>
@@ -3074,7 +3074,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1334.7</v>
+        <v>1199.2</v>
       </c>
       <c r="D98" t="n">
         <v>1106</v>
@@ -3101,7 +3101,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1008.9</v>
+        <v>4512.200000000001</v>
       </c>
       <c r="D99" t="n">
         <v>883</v>
@@ -3128,7 +3128,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>297.9</v>
+        <v>342</v>
       </c>
       <c r="D100" t="n">
         <v>336</v>
@@ -3155,7 +3155,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>368.3000000000001</v>
+        <v>413.8</v>
       </c>
       <c r="D101" t="n">
         <v>320</v>
@@ -3182,7 +3182,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1046.1</v>
+        <v>799.8</v>
       </c>
       <c r="D102" t="n">
         <v>987</v>
@@ -3209,7 +3209,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>260</v>
+        <v>313</v>
       </c>
       <c r="D103" t="n">
         <v>200</v>
@@ -3236,7 +3236,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>142.08</v>
+        <v>146.4</v>
       </c>
       <c r="D104" t="n">
         <v>149</v>
@@ -3263,7 +3263,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>534.6600000000001</v>
+        <v>1863.2</v>
       </c>
       <c r="D105" t="n">
         <v>595</v>
@@ -3290,7 +3290,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>120.2</v>
+        <v>103</v>
       </c>
       <c r="D106" t="n">
         <v>97</v>
@@ -3317,7 +3317,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>6.880000000000001</v>
+        <v>4</v>
       </c>
       <c r="D107" t="n">
         <v>8</v>
@@ -3344,7 +3344,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>200.9</v>
+        <v>171.2</v>
       </c>
       <c r="D108" t="n">
         <v>176</v>
@@ -3371,7 +3371,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>42.48</v>
+        <v>7</v>
       </c>
       <c r="D109" t="n">
         <v>68</v>
@@ -3398,7 +3398,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>331.0000000000001</v>
+        <v>251</v>
       </c>
       <c r="D110" t="n">
         <v>410</v>
@@ -3425,7 +3425,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>208.9</v>
+        <v>245</v>
       </c>
       <c r="D111" t="n">
         <v>179</v>
@@ -3452,7 +3452,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>109.6</v>
+        <v>100.2</v>
       </c>
       <c r="D112" t="n">
         <v>93</v>
@@ -3479,7 +3479,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>50.7</v>
+        <v>39.2</v>
       </c>
       <c r="D113" t="n">
         <v>39</v>
@@ -3506,7 +3506,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>20.92</v>
+        <v>21.6</v>
       </c>
       <c r="D114" t="n">
         <v>22</v>
@@ -3533,7 +3533,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>11.9</v>
+        <v>24</v>
       </c>
       <c r="D115" t="n">
         <v>17</v>
@@ -3560,7 +3560,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>22.4</v>
+        <v>24</v>
       </c>
       <c r="D116" t="n">
         <v>18</v>
@@ -3587,7 +3587,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D117" t="n">
         <v>45</v>
@@ -3614,7 +3614,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>5.6</v>
+        <v>10.4</v>
       </c>
       <c r="D118" t="n">
         <v>8</v>
@@ -3641,7 +3641,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>49.40000000000001</v>
+        <v>48</v>
       </c>
       <c r="D119" t="n">
         <v>38</v>
@@ -3668,7 +3668,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>13.3</v>
+        <v>17.6</v>
       </c>
       <c r="D120" t="n">
         <v>18</v>
@@ -3695,7 +3695,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>48.1</v>
+        <v>38.40000000000001</v>
       </c>
       <c r="D121" t="n">
         <v>37</v>

</xml_diff>